<commit_message>
Added 2018 NFL Week 5 forecasts
</commit_message>
<xml_diff>
--- a/NFL2018/Weekly Forecasts/Week4.xlsx
+++ b/NFL2018/Weekly Forecasts/Week4.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="71">
   <si>
     <t>City</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>Glendale</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>East Rutherford</t>
   </si>
   <si>
     <t>Raiders</t>
@@ -235,7 +244,7 @@
     <numFmt numFmtId="167" formatCode="#0.0"/>
     <numFmt numFmtId="168" formatCode="#0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +383,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFCA001A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFE3C00"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -420,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +566,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF192F6B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2B887"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC4C8CB"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -617,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -697,28 +726,34 @@
     <xf numFmtId="0" fontId="16" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1064,7 +1099,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.3276337967385411</v>
+        <v>0.3275786333878279</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1073,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>24.09109892211025</v>
+        <v>24.08704272964129</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -1082,10 +1117,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.9399524120095176</v>
+        <v>0.9399663120067376</v>
       </c>
       <c r="C6" s="6">
-        <v>0.0600475879904824</v>
+        <v>0.0600336879932624</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -1093,10 +1128,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>32.93246221350756</v>
+        <v>32.93000241399952</v>
       </c>
       <c r="C7" s="7">
-        <v>9.030312593937481</v>
+        <v>9.02240519551896</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -1496,35 +1531,35 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.9976995273990952</v>
+        <v>0.9977349401806967</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" s="5">
-        <v>0.7968181925330478</v>
+        <v>0.7965275407784712</v>
       </c>
       <c r="F4" s="5"/>
       <c r="H4" s="5">
-        <v>0.9998656871209395</v>
+        <v>0.9998425663504529</v>
       </c>
       <c r="I4" s="5"/>
       <c r="K4" s="5">
-        <v>0.9288404811633477</v>
+        <v>0.9290081701015783</v>
       </c>
       <c r="L4" s="5"/>
       <c r="N4" s="5">
-        <v>0.9270618456080078</v>
+        <v>0.9266116108554461</v>
       </c>
       <c r="O4" s="5"/>
       <c r="Q4" s="5">
-        <v>0.9690580115183907</v>
+        <v>0.9687694016026516</v>
       </c>
       <c r="R4" s="5"/>
       <c r="T4" s="5">
-        <v>0.9681021057031729</v>
+        <v>0.9679173253673456</v>
       </c>
       <c r="U4" s="5"/>
       <c r="W4" s="5">
-        <v>0.9299709475709748</v>
+        <v>0.9299120313053085</v>
       </c>
       <c r="X4" s="5"/>
     </row>
@@ -1533,35 +1568,35 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>54.01385627300851</v>
+        <v>54.01577346435032</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="4">
-        <v>22.92991974356349</v>
+        <v>22.92155570083929</v>
       </c>
       <c r="F5" s="4"/>
       <c r="H5" s="4">
-        <v>56.56115314825843</v>
+        <v>56.55984523514846</v>
       </c>
       <c r="I5" s="4"/>
       <c r="K5" s="4">
-        <v>55.30387356240993</v>
+        <v>55.3138578902098</v>
       </c>
       <c r="L5" s="4"/>
       <c r="N5" s="4">
-        <v>38.747752900136</v>
+        <v>38.72893475437586</v>
       </c>
       <c r="O5" s="4"/>
       <c r="Q5" s="4">
-        <v>41.14658547147189</v>
+        <v>41.13433098059031</v>
       </c>
       <c r="R5" s="4"/>
       <c r="T5" s="4">
-        <v>35.18795289528351</v>
+        <v>35.18123661844167</v>
       </c>
       <c r="U5" s="4"/>
       <c r="W5" s="4">
-        <v>47.0223460068616</v>
+        <v>47.0193670094673</v>
       </c>
       <c r="X5" s="4"/>
     </row>
@@ -1570,52 +1605,52 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.4717713056457389</v>
+        <v>0.4719893056021389</v>
       </c>
       <c r="C6" s="6">
-        <v>0.5282286943542611</v>
+        <v>0.5280106943978611</v>
       </c>
       <c r="E6" s="6">
-        <v>0.2410718517856296</v>
+        <v>0.2408962518207496</v>
       </c>
       <c r="F6" s="6">
-        <v>0.7589281482143704</v>
+        <v>0.7591037481792504</v>
       </c>
       <c r="H6" s="6">
-        <v>0.5068225986354803</v>
+        <v>0.5073864985227003</v>
       </c>
       <c r="I6" s="6">
-        <v>0.4931774013645197</v>
+        <v>0.4926135014772997</v>
       </c>
       <c r="K6" s="6">
-        <v>0.6557362688527463</v>
+        <v>0.6555557688888463</v>
       </c>
       <c r="L6" s="6">
-        <v>0.3442637311472538</v>
+        <v>0.3444442311111538</v>
       </c>
       <c r="N6" s="6">
-        <v>0.6576371684725663</v>
+        <v>0.6581144683771063</v>
       </c>
       <c r="O6" s="6">
-        <v>0.3423628315274337</v>
+        <v>0.3418855316228937</v>
       </c>
       <c r="Q6" s="6">
-        <v>0.6031832793633441</v>
+        <v>0.6036598792680241</v>
       </c>
       <c r="R6" s="6">
-        <v>0.3968167206366559</v>
+        <v>0.3963401207319758</v>
       </c>
       <c r="T6" s="6">
-        <v>0.3952467209506558</v>
+        <v>0.3949460210107958</v>
       </c>
       <c r="U6" s="6">
-        <v>0.6047532790493442</v>
+        <v>0.6050539789892042</v>
       </c>
       <c r="W6" s="6">
-        <v>0.3454849309030138</v>
+        <v>0.3454210309157938</v>
       </c>
       <c r="X6" s="6">
-        <v>0.6545150690969862</v>
+        <v>0.6545789690842062</v>
       </c>
     </row>
     <row r="7" spans="1:67">
@@ -1623,52 +1658,52 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>16.56611428677714</v>
+        <v>16.56858328628334</v>
       </c>
       <c r="C7" s="7">
-        <v>17.55940608811878</v>
+        <v>17.5607484878503</v>
       </c>
       <c r="E7" s="7">
-        <v>17.71997785600443</v>
+        <v>17.71508985698203</v>
       </c>
       <c r="F7" s="7">
-        <v>29.69920226015955</v>
+        <v>29.70025025994995</v>
       </c>
       <c r="H7" s="7">
-        <v>12.27761634447673</v>
+        <v>12.28129914374017</v>
       </c>
       <c r="I7" s="7">
-        <v>12.12128617574277</v>
+        <v>12.12533417493317</v>
       </c>
       <c r="K7" s="7">
-        <v>25.27705654458869</v>
+        <v>25.27397734520453</v>
       </c>
       <c r="L7" s="7">
-        <v>18.92949141410172</v>
+        <v>18.93084821383036</v>
       </c>
       <c r="N7" s="7">
-        <v>29.04955619008876</v>
+        <v>29.07015378596924</v>
       </c>
       <c r="O7" s="7">
-        <v>21.76766224646755</v>
+        <v>21.76681144663771</v>
       </c>
       <c r="Q7" s="7">
-        <v>22.14528177094365</v>
+        <v>22.16003056799389</v>
       </c>
       <c r="R7" s="7">
-        <v>18.12884437423113</v>
+        <v>18.12395537520893</v>
       </c>
       <c r="T7" s="7">
-        <v>25.31741933651613</v>
+        <v>25.31183473763305</v>
       </c>
       <c r="U7" s="7">
-        <v>30.22758035448393</v>
+        <v>30.23032695393461</v>
       </c>
       <c r="W7" s="7">
-        <v>27.53331709333658</v>
+        <v>27.52696989460602</v>
       </c>
       <c r="X7" s="7">
-        <v>35.54427789114443</v>
+        <v>35.53564689287062</v>
       </c>
     </row>
     <row r="8" spans="1:67">
@@ -1888,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="8">
         <v>10</v>
@@ -2209,7 +2244,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="8">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="8">
         <v>17</v>
@@ -2545,7 +2580,7 @@
         <v>38</v>
       </c>
       <c r="L24" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N24" s="8">
         <v>43</v>
@@ -2731,9 +2766,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="2" max="12" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="0.85546875" customWidth="1"/>
     <col min="7" max="7" width="0.85546875" customWidth="1"/>
+    <col min="10" max="10" width="0.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
@@ -2755,10 +2791,16 @@
       <c r="I1" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="M1" t="s">
+      <c r="K1" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
       <c r="BI1" t="s">
@@ -2781,6 +2823,10 @@
         <v>61</v>
       </c>
       <c r="I2" s="4"/>
+      <c r="K2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:61">
       <c r="A3" s="3" t="s">
@@ -2791,69 +2837,87 @@
       </c>
       <c r="C3" s="5"/>
       <c r="E3" s="5">
-        <v>0.4768436065735576</v>
+        <v>0.392474931410328</v>
       </c>
       <c r="F3" s="5"/>
       <c r="H3" s="5">
+        <v>0.4768436065735576</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="K3" s="5">
         <v>0.5889823309763212</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:61">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.7773232363840202</v>
+        <v>0.7776495033332599</v>
       </c>
       <c r="C4" s="5"/>
       <c r="E4" s="5">
-        <v>0.9154663785370194</v>
+        <v>0.9850859678549155</v>
       </c>
       <c r="F4" s="5"/>
       <c r="H4" s="5">
-        <v>0.9483919344952392</v>
+        <v>0.9151614287564427</v>
       </c>
       <c r="I4" s="5"/>
+      <c r="K4" s="5">
+        <v>0.9485712212403479</v>
+      </c>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:61">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>23.76465785703188</v>
+        <v>23.77463262950209</v>
       </c>
       <c r="C5" s="4"/>
       <c r="E5" s="4">
-        <v>43.65342896384261</v>
+        <v>38.66215476671346</v>
       </c>
       <c r="F5" s="4"/>
       <c r="H5" s="4">
-        <v>55.85860922581485</v>
+        <v>43.6388876285232</v>
       </c>
       <c r="I5" s="4"/>
+      <c r="K5" s="4">
+        <v>55.86916889831958</v>
+      </c>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:61">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.2296056540788692</v>
+        <v>0.2297925540414892</v>
       </c>
       <c r="C6" s="6">
-        <v>0.7703943459211308</v>
+        <v>0.7702074459585108</v>
       </c>
       <c r="E6" s="6">
-        <v>0.3305294338941132</v>
+        <v>0.4282297143540572</v>
       </c>
       <c r="F6" s="6">
-        <v>0.6694705661058867</v>
+        <v>0.5717702856459429</v>
       </c>
       <c r="H6" s="6">
-        <v>0.6329348734130253</v>
+        <v>0.3302302339539532</v>
       </c>
       <c r="I6" s="6">
-        <v>0.3670651265869747</v>
+        <v>0.6697697660460468</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.6327065734586853</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.3672934265413147</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -2861,22 +2925,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>11.71182965763407</v>
+        <v>11.70579305884139</v>
       </c>
       <c r="C7" s="7">
-        <v>22.69757186048563</v>
+        <v>22.69231526153695</v>
       </c>
       <c r="E7" s="7">
-        <v>13.66447106710579</v>
+        <v>29.61981787603643</v>
       </c>
       <c r="F7" s="7">
-        <v>19.67750246449951</v>
+        <v>33.14296657140669</v>
       </c>
       <c r="H7" s="7">
-        <v>30.91552161689568</v>
+        <v>13.66927146614571</v>
       </c>
       <c r="I7" s="7">
-        <v>24.55860988827802</v>
+        <v>19.68599646280071</v>
+      </c>
+      <c r="K7" s="7">
+        <v>30.9170240165952</v>
+      </c>
+      <c r="L7" s="7">
+        <v>24.5669834866033</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -2890,15 +2960,21 @@
         <v>6</v>
       </c>
       <c r="E8" s="8">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8">
+        <v>12</v>
+      </c>
+      <c r="H8" s="8">
         <v>0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="I8" s="8">
         <v>6</v>
       </c>
-      <c r="H8" s="8">
+      <c r="K8" s="8">
         <v>10</v>
       </c>
-      <c r="I8" s="8">
+      <c r="L8" s="8">
         <v>6</v>
       </c>
     </row>
@@ -2913,15 +2989,21 @@
         <v>7</v>
       </c>
       <c r="E9" s="8">
+        <v>13</v>
+      </c>
+      <c r="F9" s="8">
+        <v>16</v>
+      </c>
+      <c r="H9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="8">
+      <c r="I9" s="8">
         <v>7</v>
       </c>
-      <c r="H9" s="8">
+      <c r="K9" s="8">
         <v>14</v>
       </c>
-      <c r="I9" s="8">
+      <c r="L9" s="8">
         <v>10</v>
       </c>
     </row>
@@ -2936,15 +3018,21 @@
         <v>10</v>
       </c>
       <c r="E10" s="8">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8">
+        <v>19</v>
+      </c>
+      <c r="H10" s="8">
         <v>6</v>
       </c>
-      <c r="F10" s="8">
+      <c r="I10" s="8">
         <v>9</v>
       </c>
-      <c r="H10" s="8">
+      <c r="K10" s="8">
         <v>16</v>
       </c>
-      <c r="I10" s="8">
+      <c r="L10" s="8">
         <v>13</v>
       </c>
     </row>
@@ -2959,15 +3047,21 @@
         <v>13</v>
       </c>
       <c r="E11" s="8">
+        <v>18</v>
+      </c>
+      <c r="F11" s="8">
+        <v>21</v>
+      </c>
+      <c r="H11" s="8">
         <v>6</v>
       </c>
-      <c r="F11" s="8">
+      <c r="I11" s="8">
         <v>10</v>
       </c>
-      <c r="H11" s="8">
+      <c r="K11" s="8">
         <v>19</v>
       </c>
-      <c r="I11" s="8">
+      <c r="L11" s="8">
         <v>14</v>
       </c>
     </row>
@@ -2982,15 +3076,21 @@
         <v>14</v>
       </c>
       <c r="E12" s="8">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8">
+        <v>23</v>
+      </c>
+      <c r="H12" s="8">
         <v>7</v>
       </c>
-      <c r="F12" s="8">
+      <c r="I12" s="8">
         <v>12</v>
       </c>
-      <c r="H12" s="8">
+      <c r="K12" s="8">
         <v>21</v>
       </c>
-      <c r="I12" s="8">
+      <c r="L12" s="8">
         <v>16</v>
       </c>
     </row>
@@ -3005,15 +3105,21 @@
         <v>16</v>
       </c>
       <c r="E13" s="8">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8">
+        <v>25</v>
+      </c>
+      <c r="H13" s="8">
         <v>9</v>
       </c>
-      <c r="F13" s="8">
+      <c r="I13" s="8">
         <v>13</v>
       </c>
-      <c r="H13" s="8">
+      <c r="K13" s="8">
         <v>23</v>
       </c>
-      <c r="I13" s="8">
+      <c r="L13" s="8">
         <v>17</v>
       </c>
     </row>
@@ -3028,15 +3134,21 @@
         <v>17</v>
       </c>
       <c r="E14" s="8">
+        <v>23</v>
+      </c>
+      <c r="F14" s="8">
+        <v>27</v>
+      </c>
+      <c r="H14" s="8">
         <v>10</v>
       </c>
-      <c r="F14" s="8">
+      <c r="I14" s="8">
         <v>15</v>
       </c>
-      <c r="H14" s="8">
+      <c r="K14" s="8">
         <v>24</v>
       </c>
-      <c r="I14" s="8">
+      <c r="L14" s="8">
         <v>19</v>
       </c>
     </row>
@@ -3051,15 +3163,21 @@
         <v>19</v>
       </c>
       <c r="E15" s="8">
+        <v>25</v>
+      </c>
+      <c r="F15" s="8">
+        <v>29</v>
+      </c>
+      <c r="H15" s="8">
         <v>10</v>
       </c>
-      <c r="F15" s="8">
+      <c r="I15" s="8">
         <v>16</v>
       </c>
-      <c r="H15" s="8">
+      <c r="K15" s="8">
         <v>26</v>
       </c>
-      <c r="I15" s="8">
+      <c r="L15" s="8">
         <v>20</v>
       </c>
     </row>
@@ -3074,19 +3192,25 @@
         <v>20</v>
       </c>
       <c r="E16" s="8">
+        <v>27</v>
+      </c>
+      <c r="F16" s="8">
+        <v>30</v>
+      </c>
+      <c r="H16" s="8">
         <v>12</v>
       </c>
-      <c r="F16" s="8">
+      <c r="I16" s="8">
         <v>17</v>
       </c>
-      <c r="H16" s="8">
+      <c r="K16" s="8">
         <v>28</v>
       </c>
-      <c r="I16" s="8">
+      <c r="L16" s="8">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:12">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -3097,19 +3221,25 @@
         <v>21</v>
       </c>
       <c r="E17" s="8">
+        <v>29</v>
+      </c>
+      <c r="F17" s="8">
+        <v>32</v>
+      </c>
+      <c r="H17" s="8">
         <v>13</v>
       </c>
-      <c r="F17" s="8">
+      <c r="I17" s="8">
         <v>19</v>
       </c>
-      <c r="H17" s="8">
+      <c r="K17" s="8">
         <v>30</v>
       </c>
-      <c r="I17" s="8">
+      <c r="L17" s="8">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:12">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -3120,19 +3250,25 @@
         <v>24</v>
       </c>
       <c r="E18" s="8">
+        <v>30</v>
+      </c>
+      <c r="F18" s="8">
+        <v>34</v>
+      </c>
+      <c r="H18" s="8">
         <v>13</v>
       </c>
-      <c r="F18" s="8">
+      <c r="I18" s="8">
         <v>20</v>
       </c>
-      <c r="H18" s="8">
+      <c r="K18" s="8">
         <v>31</v>
       </c>
-      <c r="I18" s="8">
+      <c r="L18" s="8">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:12">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -3143,19 +3279,25 @@
         <v>24</v>
       </c>
       <c r="E19" s="8">
+        <v>32</v>
+      </c>
+      <c r="F19" s="8">
+        <v>36</v>
+      </c>
+      <c r="H19" s="8">
         <v>15</v>
       </c>
-      <c r="F19" s="8">
+      <c r="I19" s="8">
         <v>22</v>
       </c>
-      <c r="H19" s="8">
+      <c r="K19" s="8">
         <v>33</v>
       </c>
-      <c r="I19" s="8">
+      <c r="L19" s="8">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:12">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -3166,19 +3308,25 @@
         <v>27</v>
       </c>
       <c r="E20" s="8">
+        <v>34</v>
+      </c>
+      <c r="F20" s="8">
+        <v>38</v>
+      </c>
+      <c r="H20" s="8">
         <v>16</v>
       </c>
-      <c r="F20" s="8">
+      <c r="I20" s="8">
         <v>23</v>
       </c>
-      <c r="H20" s="8">
+      <c r="K20" s="8">
         <v>35</v>
       </c>
-      <c r="I20" s="8">
+      <c r="L20" s="8">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:12">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -3189,19 +3337,25 @@
         <v>28</v>
       </c>
       <c r="E21" s="8">
+        <v>36</v>
+      </c>
+      <c r="F21" s="8">
+        <v>40</v>
+      </c>
+      <c r="H21" s="8">
         <v>17</v>
       </c>
-      <c r="F21" s="8">
+      <c r="I21" s="8">
         <v>24</v>
       </c>
-      <c r="H21" s="8">
+      <c r="K21" s="8">
         <v>37</v>
       </c>
-      <c r="I21" s="8">
+      <c r="L21" s="8">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:12">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -3212,19 +3366,25 @@
         <v>31</v>
       </c>
       <c r="E22" s="8">
+        <v>38</v>
+      </c>
+      <c r="F22" s="8">
+        <v>42</v>
+      </c>
+      <c r="H22" s="8">
         <v>19</v>
       </c>
-      <c r="F22" s="8">
+      <c r="I22" s="8">
         <v>26</v>
       </c>
-      <c r="H22" s="8">
+      <c r="K22" s="8">
         <v>40</v>
       </c>
-      <c r="I22" s="8">
+      <c r="L22" s="8">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:12">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -3235,19 +3395,25 @@
         <v>32</v>
       </c>
       <c r="E23" s="8">
+        <v>41</v>
+      </c>
+      <c r="F23" s="8">
+        <v>45</v>
+      </c>
+      <c r="H23" s="8">
         <v>20</v>
       </c>
-      <c r="F23" s="8">
+      <c r="I23" s="8">
         <v>28</v>
       </c>
-      <c r="H23" s="8">
+      <c r="K23" s="8">
         <v>42</v>
       </c>
-      <c r="I23" s="8">
+      <c r="L23" s="8">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:12">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -3258,19 +3424,25 @@
         <v>35</v>
       </c>
       <c r="E24" s="8">
+        <v>44</v>
+      </c>
+      <c r="F24" s="8">
+        <v>48</v>
+      </c>
+      <c r="H24" s="8">
         <v>23</v>
       </c>
-      <c r="F24" s="8">
+      <c r="I24" s="8">
         <v>30</v>
       </c>
-      <c r="H24" s="8">
+      <c r="K24" s="8">
         <v>45</v>
       </c>
-      <c r="I24" s="8">
+      <c r="L24" s="8">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:12">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -3281,19 +3453,25 @@
         <v>38</v>
       </c>
       <c r="E25" s="8">
+        <v>48</v>
+      </c>
+      <c r="F25" s="8">
+        <v>52</v>
+      </c>
+      <c r="H25" s="8">
         <v>26</v>
       </c>
-      <c r="F25" s="8">
+      <c r="I25" s="8">
         <v>33</v>
       </c>
-      <c r="H25" s="8">
+      <c r="K25" s="8">
         <v>50</v>
       </c>
-      <c r="I25" s="8">
+      <c r="L25" s="8">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:12">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -3304,20 +3482,26 @@
         <v>45</v>
       </c>
       <c r="E26" s="8">
+        <v>54</v>
+      </c>
+      <c r="F26" s="8">
+        <v>58</v>
+      </c>
+      <c r="H26" s="8">
         <v>30</v>
       </c>
-      <c r="F26" s="8">
+      <c r="I26" s="8">
         <v>38</v>
       </c>
-      <c r="H26" s="8">
+      <c r="K26" s="8">
         <v>56</v>
       </c>
-      <c r="I26" s="8">
+      <c r="L26" s="8">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -3330,6 +3514,10 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3353,11 +3541,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="B1" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>63</v>
+      <c r="B1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="BI1" t="s">
         <v>28</v>
@@ -3368,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -3386,7 +3574,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.831206374229674</v>
+        <v>0.8312389326780074</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -3395,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>50.78307245975546</v>
+        <v>50.7850616384867</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3404,10 +3592,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.2629775474044905</v>
+        <v>0.2629994474001105</v>
       </c>
       <c r="C6" s="6">
-        <v>0.7370224525955095</v>
+        <v>0.7370005525998895</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -3415,10 +3603,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>22.12934557413088</v>
+        <v>22.1274739745052</v>
       </c>
       <c r="C7" s="7">
-        <v>34.40651531869694</v>
+        <v>34.39632272073545</v>
       </c>
     </row>
     <row r="8" spans="1:61">
@@ -3659,11 +3847,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
-      <c r="B1" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>66</v>
+      <c r="B1" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>69</v>
       </c>
       <c r="BI1" t="s">
         <v>28</v>
@@ -3674,7 +3862,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -3692,7 +3880,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.9078605424275206</v>
+        <v>0.9078483884878005</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -3701,7 +3889,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>42.64206322092021</v>
+        <v>42.64149235233224</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -3710,10 +3898,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0.3232310353537929</v>
+        <v>0.323219635356073</v>
       </c>
       <c r="C6" s="6">
-        <v>0.6767689646462071</v>
+        <v>0.6767803646439271</v>
       </c>
     </row>
     <row r="7" spans="1:61">
@@ -3721,10 +3909,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>26.18762896247421</v>
+        <v>26.18666076266785</v>
       </c>
       <c r="C7" s="7">
-        <v>35.29088514182297</v>
+        <v>35.28775434244913</v>
       </c>
     </row>
     <row r="8" spans="1:61">

</xml_diff>